<commit_message>
metadata pipeline logs and staging updates
</commit_message>
<xml_diff>
--- a/metadata/study_descriptions.xlsx
+++ b/metadata/study_descriptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kspann/Desktop/HMO Power Bi/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC6D6694-2D0F-1943-BF26-0DE439309B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95973027-AD1A-7944-AF2B-F4D20219D13F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="3080" windowWidth="25820" windowHeight="13200" xr2:uid="{C565C667-849D-9249-AB27-87AD06C85CD3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>StudyID</t>
   </si>
@@ -60,6 +60,60 @@
   </si>
   <si>
     <t>Hormonal influence on HMO composition from colostrum to mature milk</t>
+  </si>
+  <si>
+    <t>Keywords</t>
+  </si>
+  <si>
+    <t>colostrum; hormones; early postpartum</t>
+  </si>
+  <si>
+    <t>supplements</t>
+  </si>
+  <si>
+    <t>NICU; donor milk; preterm</t>
+  </si>
+  <si>
+    <t>DHM Pooled</t>
+  </si>
+  <si>
+    <t>Looking at single donor profiles and paired samples (pre-post)</t>
+  </si>
+  <si>
+    <t>Milk Banks</t>
+  </si>
+  <si>
+    <t>collection window</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Days 1-5 Postpartum &amp; 24days+ </t>
+  </si>
+  <si>
+    <t>varied</t>
+  </si>
+  <si>
+    <t>NICU stay</t>
+  </si>
+  <si>
+    <t>population</t>
+  </si>
+  <si>
+    <t>donor milk only</t>
+  </si>
+  <si>
+    <t>preterm NICU infants</t>
+  </si>
+  <si>
+    <t>term infants</t>
+  </si>
+  <si>
+    <t>sample type</t>
+  </si>
+  <si>
+    <t>colostrum, transitional, mature milk</t>
+  </si>
+  <si>
+    <t>donor human milk (pooled)</t>
   </si>
 </sst>
 </file>
@@ -431,44 +485,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{834A080E-18F9-DD4F-9B3D-16F44043D077}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="76.5" customWidth="1"/>
+    <col min="3" max="3" width="38.33203125" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>